<commit_message>
Update Stress Fatigue Factor.xlsx
</commit_message>
<xml_diff>
--- a/Data Files/Stress Fatigue Factor.xlsx
+++ b/Data Files/Stress Fatigue Factor.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab R202a\bin\Matlab Projects\Gear Designer\GD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab R202a\bin\Matlab Projects\Gear Designer\Spur Gear Designer\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Average_BHN_steel</t>
   </si>
@@ -44,12 +43,6 @@
   </si>
   <si>
     <t>Cast Iron</t>
-  </si>
-  <si>
-    <t>Bronze</t>
-  </si>
-  <si>
-    <t>Material</t>
   </si>
 </sst>
 </file>
@@ -106,9 +99,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -475,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -538,83 +534,19 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>150</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1">
-        <v>317</v>
-      </c>
-      <c r="D5" s="1">
-        <v>427</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>200</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1">
-        <v>503</v>
-      </c>
-      <c r="D6" s="1">
-        <v>689</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1050</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1420</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1330</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1960</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>